<commit_message>
Test Data excel changes - 11 Oct 2023
</commit_message>
<xml_diff>
--- a/TestData/TS04AndTS07_ValidateERPSection2.xlsx
+++ b/TestData/TS04AndTS07_ValidateERPSection2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgoyal0427\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE5E643-2CCC-4DD4-AADD-17B7D212E7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7530"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddOpportunity" sheetId="1" r:id="rId1"/>
@@ -23,20 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="90">
   <si>
     <t>Client</t>
   </si>
@@ -301,12 +294,18 @@
   <si>
     <t xml:space="preserve"> 
 Debt Capital Markets</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>10000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -365,11 +364,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -377,7 +374,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -659,408 +656,403 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="3"/>
-    <col min="15" max="17" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="27" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="8.85546875" style="3"/>
-    <col min="26" max="26" width="11.28515625" style="3" customWidth="1"/>
-    <col min="27" max="30" width="8.85546875" style="3"/>
-    <col min="31" max="31" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="14.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.33203125" customWidth="1"/>
+    <col min="31" max="31" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" t="s">
         <v>56</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="R2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" t="s">
+        <v>29</v>
+      </c>
+      <c r="V2" t="s">
+        <v>58</v>
+      </c>
+      <c r="W2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" t="s">
+        <v>86</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R3" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S3" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U3" t="s">
         <v>29</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V3" t="s">
         <v>58</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W3" t="s">
         <v>32</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X3" t="s">
         <v>34</v>
       </c>
-      <c r="Y2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Y3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z3" t="s">
         <v>43</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AA3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AB3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AC2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF2"/>
-    </row>
-    <row r="3" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="AD3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="3" t="s">
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L4" t="s">
         <v>56</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA3" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" t="s">
         <v>18</v>
       </c>
       <c r="N4" t="s">
         <v>73</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="R4" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="S4" t="s">
         <v>26</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="T4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="U4" t="s">
         <v>29</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="V4" t="s">
         <v>58</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="W4" t="s">
         <v>32</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="X4" t="s">
         <v>34</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Y4" t="s">
         <v>74</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="Z4" t="s">
         <v>43</v>
       </c>
-      <c r="AA4" s="5" t="s">
+      <c r="AA4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AB4" s="5" t="s">
+      <c r="AB4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AD4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1071,20 +1063,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1092,7 +1084,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1100,7 +1092,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -1108,7 +1100,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1122,22 +1114,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>67</v>
       </c>
@@ -1154,7 +1146,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -1178,24 +1170,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -1221,7 +1213,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1254,21 +1246,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
@@ -1279,7 +1271,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>64</v>
       </c>

</xml_diff>